<commit_message>
Dec 17th 5th Commit
</commit_message>
<xml_diff>
--- a/20211213 KPI_ACTION_TRACKER.xlsx
+++ b/20211213 KPI_ACTION_TRACKER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\usat-dfs\INTL\MYPB\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Alcon.net\MYPB-DFS\DATA\AL\BusUnits\Alcon GSC FRA Ops\01 R2P\00. R2P General\JPN &amp; KOR\01 TEAM_BUILDING\01 TEAM MEETING\DAILY HUDDLE MEETING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3997381E-8953-4950-8354-BBC0EC5A71B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2C39AA-6D44-42E2-AA4F-6C29E088F62B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,10 +19,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">KPI!$A$1:$G$23</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -86,23 +95,11 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>What(Action Items)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>POT% is not meeting 100% even though we are on target(over 80%).</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Nizam, Hakimi &amp; Hanis</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Who(Responsible)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>When(Due date)</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
@@ -194,14 +191,6 @@
   </si>
   <si>
     <t>Appzen Configuration setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Have to discuss further with IT representative
-</t>
-  </si>
-  <si>
-    <t>1. Need discussion with Yamazaki-san and other party to solve user's question
-2. Send VoC survey after providing answers to users</t>
   </si>
   <si>
     <t>C &amp; B analysis - Relocation fees process alignment</t>
@@ -354,6 +343,23 @@
   <si>
     <t>1. Informing all users of Korea of the new method of query submission via email with translated how-to guide - by end of Dec. 2021
 2. Giving consistent guide of the change to users via email and messages whenever contacted -end of Jan. 2022</t>
+  </si>
+  <si>
+    <t>1. Need discussion with Yamazaki-san and other party to solve user's question by end of December
+2. Send one VoC survey after providing answers to users by end of January 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Have to discuss further with IT representative by mid of January
+</t>
+  </si>
+  <si>
+    <t>What_Action_Items</t>
+  </si>
+  <si>
+    <t>Who_Responsible</t>
+  </si>
+  <si>
+    <t>When_Due_date</t>
   </si>
 </sst>
 </file>
@@ -772,7 +778,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -790,16 +796,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>88</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
@@ -816,16 +822,16 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>8</v>
@@ -836,19 +842,19 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>8</v>
@@ -859,17 +865,17 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>8</v>
@@ -880,20 +886,20 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="43.5">
@@ -901,17 +907,17 @@
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>8</v>
@@ -922,38 +928,38 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.5">
+      <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="29">
-      <c r="A8" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>8</v>
@@ -961,22 +967,22 @@
     </row>
     <row r="9" spans="1:7" ht="87">
       <c r="A9" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>8</v>
@@ -984,22 +990,22 @@
     </row>
     <row r="10" spans="1:7" ht="217.5">
       <c r="A10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>8</v>
@@ -1007,22 +1013,22 @@
     </row>
     <row r="11" spans="1:7" ht="159.5">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>8</v>
@@ -1030,20 +1036,20 @@
     </row>
     <row r="12" spans="1:7" ht="29">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>8</v>
@@ -1051,22 +1057,22 @@
     </row>
     <row r="13" spans="1:7" ht="72.5">
       <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>8</v>
@@ -1074,22 +1080,22 @@
     </row>
     <row r="14" spans="1:7" ht="58">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="F14" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>8</v>
@@ -1097,20 +1103,20 @@
     </row>
     <row r="15" spans="1:7" ht="29">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>8</v>
@@ -1118,20 +1124,20 @@
     </row>
     <row r="16" spans="1:7" ht="29">
       <c r="A16" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>8</v>
@@ -1139,20 +1145,20 @@
     </row>
     <row r="17" spans="1:7" ht="29">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>8</v>
@@ -1160,20 +1166,20 @@
     </row>
     <row r="18" spans="1:7" ht="29">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>8</v>
@@ -1181,20 +1187,20 @@
     </row>
     <row r="19" spans="1:7" ht="43.5">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>8</v>
@@ -1202,20 +1208,20 @@
     </row>
     <row r="20" spans="1:7" ht="43.5">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>8</v>
@@ -1223,41 +1229,41 @@
     </row>
     <row r="21" spans="1:7" ht="29">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="29">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>8</v>
@@ -1265,20 +1271,20 @@
     </row>
     <row r="23" spans="1:7" ht="29">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>8</v>
@@ -1286,20 +1292,20 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>8</v>
@@ -1307,22 +1313,22 @@
     </row>
     <row r="25" spans="1:7" ht="39" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>8</v>
@@ -1330,22 +1336,22 @@
     </row>
     <row r="26" spans="1:7" ht="35.5" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>8</v>
@@ -1353,20 +1359,20 @@
     </row>
     <row r="27" spans="1:7" ht="58">
       <c r="A27" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>8</v>

</xml_diff>